<commit_message>
Final supplementary material added
</commit_message>
<xml_diff>
--- a/Coded_texts.xlsx
+++ b/Coded_texts.xlsx
@@ -29,9 +29,9 @@
   </sheets>
   <calcPr calcId="162913"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId15"/>
-    <pivotCache cacheId="1" r:id="rId16"/>
-    <pivotCache cacheId="2" r:id="rId17"/>
+    <pivotCache cacheId="4" r:id="rId15"/>
+    <pivotCache cacheId="5" r:id="rId16"/>
+    <pivotCache cacheId="6" r:id="rId17"/>
   </pivotCaches>
 </workbook>
 </file>
@@ -4612,30 +4612,73 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="28" fillId="3" borderId="1" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="35" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="29" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="1" xfId="6" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="1" xfId="6" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="1" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="1" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="1" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="1" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="1" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="1" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="1" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="1" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="34" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="35" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="33" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="1" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="1" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="1" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="1" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="35" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="33" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="28" borderId="1" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -4643,49 +4686,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="28" borderId="1" xfId="6" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="33" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="33" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="34" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="1" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="1" xfId="7" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="1" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="1" xfId="7" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="3" borderId="1" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="1" xfId="6" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="1" xfId="6" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="26" borderId="16" xfId="4"/>
     <xf numFmtId="0" fontId="1" fillId="29" borderId="12" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -4736,16 +4736,16 @@
     <xf numFmtId="0" fontId="1" fillId="27" borderId="5" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="19" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="20" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="21" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="12">
     <cellStyle name="20% - Accent4" xfId="7" builtinId="42"/>
@@ -5601,6 +5601,62 @@
           <a:effectLst/>
         </c:spPr>
       </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="10"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="11"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="12"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="13"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
     </c:pivotFmts>
     <c:plotArea>
       <c:layout/>
@@ -6087,6 +6143,34 @@
       </c:pivotFmt>
       <c:pivotFmt>
         <c:idx val="4"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="5"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="6"/>
         <c:spPr>
           <a:solidFill>
             <a:schemeClr val="accent1"/>
@@ -8270,7 +8354,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable5" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="16">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable5" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="16">
   <location ref="A3:B9" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="2">
     <pivotField axis="axisRow" showAll="0">
@@ -8395,7 +8479,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="12">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="12">
   <location ref="A3:B8" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="2">
     <pivotField axis="axisRow" showAll="0">
@@ -8435,12 +8519,60 @@
   <dataFields count="1">
     <dataField name="Sum of Count" fld="1" baseField="0" baseItem="0"/>
   </dataFields>
-  <chartFormats count="1">
+  <chartFormats count="5">
     <chartFormat chart="0" format="1" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
             <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="10">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="11">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="12">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="13">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="3"/>
           </reference>
         </references>
       </pivotArea>
@@ -8456,7 +8588,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="15">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="15">
   <location ref="A3:B6" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="2">
     <pivotField axis="axisRow" showAll="0">
@@ -8488,12 +8620,36 @@
   <dataFields count="1">
     <dataField name="Sum of Count" fld="1" baseField="0" baseItem="0"/>
   </dataFields>
-  <chartFormats count="1">
+  <chartFormats count="3">
     <chartFormat chart="3" format="0" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
             <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="3" format="5">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="3" format="6">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="1"/>
           </reference>
         </references>
       </pivotArea>
@@ -8720,10 +8876,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D54" sqref="D54"/>
-      <selection pane="bottomLeft" activeCell="D48" sqref="D48"/>
+      <selection pane="bottomLeft" activeCell="X17" sqref="X17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
@@ -15281,20 +15437,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="A1" s="278" t="s">
+      <c r="A1" s="256" t="s">
         <v>805</v>
       </c>
-      <c r="B1" s="278"/>
-      <c r="C1" s="278"/>
-      <c r="D1" s="278"/>
-      <c r="E1" s="278"/>
-      <c r="F1" s="278"/>
-      <c r="G1" s="278"/>
-      <c r="H1" s="278"/>
-      <c r="I1" s="278"/>
+      <c r="B1" s="256"/>
+      <c r="C1" s="256"/>
+      <c r="D1" s="256"/>
+      <c r="E1" s="256"/>
+      <c r="F1" s="256"/>
+      <c r="G1" s="256"/>
+      <c r="H1" s="256"/>
+      <c r="I1" s="256"/>
     </row>
     <row r="2" spans="1:10">
-      <c r="A2" s="279" t="s">
+      <c r="A2" s="259" t="s">
         <v>861</v>
       </c>
       <c r="B2" s="251"/>
@@ -15310,7 +15466,7 @@
       </c>
     </row>
     <row r="3" spans="1:10">
-      <c r="A3" s="279" t="s">
+      <c r="A3" s="259" t="s">
         <v>806</v>
       </c>
       <c r="B3" s="251"/>
@@ -15326,257 +15482,257 @@
       </c>
     </row>
     <row r="4" spans="1:10">
-      <c r="A4" s="259" t="s">
+      <c r="A4" s="260" t="s">
         <v>833</v>
       </c>
-      <c r="B4" s="260"/>
-      <c r="C4" s="260"/>
-      <c r="D4" s="260"/>
-      <c r="E4" s="260"/>
-      <c r="F4" s="260"/>
-      <c r="G4" s="260"/>
-      <c r="H4" s="260"/>
-      <c r="I4" s="260"/>
+      <c r="B4" s="261"/>
+      <c r="C4" s="261"/>
+      <c r="D4" s="261"/>
+      <c r="E4" s="261"/>
+      <c r="F4" s="261"/>
+      <c r="G4" s="261"/>
+      <c r="H4" s="261"/>
+      <c r="I4" s="261"/>
       <c r="J4">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="280" t="s">
+      <c r="A5" s="262" t="s">
         <v>807</v>
       </c>
-      <c r="B5" s="281"/>
-      <c r="C5" s="281"/>
-      <c r="D5" s="281"/>
-      <c r="E5" s="281"/>
-      <c r="F5" s="281"/>
-      <c r="G5" s="281"/>
-      <c r="H5" s="281"/>
-      <c r="I5" s="281"/>
+      <c r="B5" s="263"/>
+      <c r="C5" s="263"/>
+      <c r="D5" s="263"/>
+      <c r="E5" s="263"/>
+      <c r="F5" s="263"/>
+      <c r="G5" s="263"/>
+      <c r="H5" s="263"/>
+      <c r="I5" s="263"/>
       <c r="J5">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="257" t="s">
+      <c r="A6" s="264" t="s">
         <v>808</v>
       </c>
-      <c r="B6" s="282"/>
-      <c r="C6" s="282"/>
-      <c r="D6" s="282"/>
-      <c r="E6" s="282"/>
-      <c r="F6" s="282"/>
-      <c r="G6" s="282"/>
-      <c r="H6" s="282"/>
-      <c r="I6" s="282"/>
+      <c r="B6" s="265"/>
+      <c r="C6" s="265"/>
+      <c r="D6" s="265"/>
+      <c r="E6" s="265"/>
+      <c r="F6" s="265"/>
+      <c r="G6" s="265"/>
+      <c r="H6" s="265"/>
+      <c r="I6" s="265"/>
       <c r="J6">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="257" t="s">
+      <c r="A7" s="264" t="s">
         <v>809</v>
       </c>
-      <c r="B7" s="282"/>
-      <c r="C7" s="282"/>
-      <c r="D7" s="282"/>
-      <c r="E7" s="282"/>
-      <c r="F7" s="282"/>
-      <c r="G7" s="282"/>
-      <c r="H7" s="282"/>
-      <c r="I7" s="282"/>
+      <c r="B7" s="265"/>
+      <c r="C7" s="265"/>
+      <c r="D7" s="265"/>
+      <c r="E7" s="265"/>
+      <c r="F7" s="265"/>
+      <c r="G7" s="265"/>
+      <c r="H7" s="265"/>
+      <c r="I7" s="265"/>
       <c r="J7">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="259" t="s">
+      <c r="A8" s="260" t="s">
         <v>810</v>
       </c>
-      <c r="B8" s="260"/>
-      <c r="C8" s="260"/>
-      <c r="D8" s="260"/>
-      <c r="E8" s="260"/>
-      <c r="F8" s="260"/>
-      <c r="G8" s="260"/>
-      <c r="H8" s="260"/>
-      <c r="I8" s="260"/>
+      <c r="B8" s="261"/>
+      <c r="C8" s="261"/>
+      <c r="D8" s="261"/>
+      <c r="E8" s="261"/>
+      <c r="F8" s="261"/>
+      <c r="G8" s="261"/>
+      <c r="H8" s="261"/>
+      <c r="I8" s="261"/>
       <c r="J8">
         <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="259" t="s">
+      <c r="A9" s="260" t="s">
         <v>811</v>
       </c>
-      <c r="B9" s="260"/>
-      <c r="C9" s="260"/>
-      <c r="D9" s="260"/>
-      <c r="E9" s="260"/>
-      <c r="F9" s="260"/>
-      <c r="G9" s="260"/>
-      <c r="H9" s="260"/>
-      <c r="I9" s="260"/>
+      <c r="B9" s="261"/>
+      <c r="C9" s="261"/>
+      <c r="D9" s="261"/>
+      <c r="E9" s="261"/>
+      <c r="F9" s="261"/>
+      <c r="G9" s="261"/>
+      <c r="H9" s="261"/>
+      <c r="I9" s="261"/>
       <c r="J9">
         <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="261" t="s">
+      <c r="A10" s="266" t="s">
         <v>812</v>
       </c>
-      <c r="B10" s="262"/>
-      <c r="C10" s="262"/>
-      <c r="D10" s="262"/>
-      <c r="E10" s="262"/>
-      <c r="F10" s="262"/>
-      <c r="G10" s="262"/>
-      <c r="H10" s="262"/>
-      <c r="I10" s="262"/>
+      <c r="B10" s="267"/>
+      <c r="C10" s="267"/>
+      <c r="D10" s="267"/>
+      <c r="E10" s="267"/>
+      <c r="F10" s="267"/>
+      <c r="G10" s="267"/>
+      <c r="H10" s="267"/>
+      <c r="I10" s="267"/>
       <c r="J10">
         <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="31.5" customHeight="1">
-      <c r="A11" s="283" t="s">
+      <c r="A11" s="268" t="s">
         <v>813</v>
       </c>
-      <c r="B11" s="284"/>
-      <c r="C11" s="284"/>
-      <c r="D11" s="284"/>
-      <c r="E11" s="284"/>
-      <c r="F11" s="284"/>
-      <c r="G11" s="284"/>
-      <c r="H11" s="284"/>
-      <c r="I11" s="284"/>
+      <c r="B11" s="269"/>
+      <c r="C11" s="269"/>
+      <c r="D11" s="269"/>
+      <c r="E11" s="269"/>
+      <c r="F11" s="269"/>
+      <c r="G11" s="269"/>
+      <c r="H11" s="269"/>
+      <c r="I11" s="269"/>
       <c r="J11">
         <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="259" t="s">
+      <c r="A12" s="260" t="s">
         <v>814</v>
       </c>
-      <c r="B12" s="260"/>
-      <c r="C12" s="260"/>
-      <c r="D12" s="260"/>
-      <c r="E12" s="260"/>
-      <c r="F12" s="260"/>
-      <c r="G12" s="260"/>
-      <c r="H12" s="260"/>
-      <c r="I12" s="260"/>
+      <c r="B12" s="261"/>
+      <c r="C12" s="261"/>
+      <c r="D12" s="261"/>
+      <c r="E12" s="261"/>
+      <c r="F12" s="261"/>
+      <c r="G12" s="261"/>
+      <c r="H12" s="261"/>
+      <c r="I12" s="261"/>
       <c r="J12">
         <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" s="265" t="s">
+      <c r="A13" s="257" t="s">
         <v>815</v>
       </c>
-      <c r="B13" s="277"/>
-      <c r="C13" s="277"/>
-      <c r="D13" s="277"/>
-      <c r="E13" s="277"/>
-      <c r="F13" s="277"/>
-      <c r="G13" s="277"/>
-      <c r="H13" s="277"/>
-      <c r="I13" s="277"/>
+      <c r="B13" s="258"/>
+      <c r="C13" s="258"/>
+      <c r="D13" s="258"/>
+      <c r="E13" s="258"/>
+      <c r="F13" s="258"/>
+      <c r="G13" s="258"/>
+      <c r="H13" s="258"/>
+      <c r="I13" s="258"/>
       <c r="J13">
         <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:10">
-      <c r="A14" s="265" t="s">
+      <c r="A14" s="257" t="s">
         <v>816</v>
       </c>
-      <c r="B14" s="277"/>
-      <c r="C14" s="277"/>
-      <c r="D14" s="277"/>
-      <c r="E14" s="277"/>
-      <c r="F14" s="277"/>
-      <c r="G14" s="277"/>
-      <c r="H14" s="277"/>
-      <c r="I14" s="277"/>
+      <c r="B14" s="258"/>
+      <c r="C14" s="258"/>
+      <c r="D14" s="258"/>
+      <c r="E14" s="258"/>
+      <c r="F14" s="258"/>
+      <c r="G14" s="258"/>
+      <c r="H14" s="258"/>
+      <c r="I14" s="258"/>
       <c r="J14">
         <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:10">
-      <c r="A15" s="259" t="s">
+      <c r="A15" s="260" t="s">
         <v>817</v>
       </c>
-      <c r="B15" s="260"/>
-      <c r="C15" s="260"/>
-      <c r="D15" s="260"/>
-      <c r="E15" s="260"/>
-      <c r="F15" s="260"/>
-      <c r="G15" s="260"/>
-      <c r="H15" s="260"/>
-      <c r="I15" s="260"/>
+      <c r="B15" s="261"/>
+      <c r="C15" s="261"/>
+      <c r="D15" s="261"/>
+      <c r="E15" s="261"/>
+      <c r="F15" s="261"/>
+      <c r="G15" s="261"/>
+      <c r="H15" s="261"/>
+      <c r="I15" s="261"/>
       <c r="J15">
         <v>7</v>
       </c>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="277" t="s">
+      <c r="A16" s="258" t="s">
         <v>821</v>
       </c>
-      <c r="B16" s="277"/>
-      <c r="C16" s="277"/>
-      <c r="D16" s="277"/>
-      <c r="E16" s="277"/>
-      <c r="F16" s="277"/>
-      <c r="G16" s="277"/>
-      <c r="H16" s="277"/>
-      <c r="I16" s="277"/>
+      <c r="B16" s="258"/>
+      <c r="C16" s="258"/>
+      <c r="D16" s="258"/>
+      <c r="E16" s="258"/>
+      <c r="F16" s="258"/>
+      <c r="G16" s="258"/>
+      <c r="H16" s="258"/>
+      <c r="I16" s="258"/>
       <c r="J16">
         <v>7</v>
       </c>
     </row>
     <row r="17" spans="1:22">
-      <c r="A17" s="261" t="s">
+      <c r="A17" s="266" t="s">
         <v>818</v>
       </c>
-      <c r="B17" s="262"/>
-      <c r="C17" s="262"/>
-      <c r="D17" s="262"/>
-      <c r="E17" s="262"/>
-      <c r="F17" s="262"/>
-      <c r="G17" s="262"/>
-      <c r="H17" s="262"/>
-      <c r="I17" s="262"/>
+      <c r="B17" s="267"/>
+      <c r="C17" s="267"/>
+      <c r="D17" s="267"/>
+      <c r="E17" s="267"/>
+      <c r="F17" s="267"/>
+      <c r="G17" s="267"/>
+      <c r="H17" s="267"/>
+      <c r="I17" s="267"/>
       <c r="J17">
         <v>9</v>
       </c>
     </row>
     <row r="18" spans="1:22" ht="29.25" customHeight="1">
-      <c r="A18" s="275" t="s">
+      <c r="A18" s="272" t="s">
         <v>825</v>
       </c>
-      <c r="B18" s="276"/>
-      <c r="C18" s="276"/>
-      <c r="D18" s="276"/>
-      <c r="E18" s="276"/>
-      <c r="F18" s="276"/>
-      <c r="G18" s="276"/>
-      <c r="H18" s="276"/>
-      <c r="I18" s="276"/>
+      <c r="B18" s="273"/>
+      <c r="C18" s="273"/>
+      <c r="D18" s="273"/>
+      <c r="E18" s="273"/>
+      <c r="F18" s="273"/>
+      <c r="G18" s="273"/>
+      <c r="H18" s="273"/>
+      <c r="I18" s="273"/>
       <c r="J18">
         <v>9</v>
       </c>
     </row>
     <row r="19" spans="1:22">
-      <c r="A19" s="268" t="s">
+      <c r="A19" s="277" t="s">
         <v>819</v>
       </c>
-      <c r="B19" s="269"/>
-      <c r="C19" s="269"/>
-      <c r="D19" s="269"/>
-      <c r="E19" s="269"/>
-      <c r="F19" s="269"/>
-      <c r="G19" s="269"/>
-      <c r="H19" s="269"/>
-      <c r="I19" s="269"/>
+      <c r="B19" s="278"/>
+      <c r="C19" s="278"/>
+      <c r="D19" s="278"/>
+      <c r="E19" s="278"/>
+      <c r="F19" s="278"/>
+      <c r="G19" s="278"/>
+      <c r="H19" s="278"/>
+      <c r="I19" s="278"/>
       <c r="J19">
         <v>10</v>
       </c>
@@ -15596,641 +15752,599 @@
       <c r="J20">
         <v>11</v>
       </c>
-      <c r="K20" s="257" t="s">
+      <c r="K20" s="264" t="s">
         <v>822</v>
       </c>
-      <c r="L20" s="257"/>
-      <c r="M20" s="257"/>
-      <c r="N20" s="257"/>
-      <c r="O20" s="257"/>
-      <c r="P20" s="257"/>
-      <c r="Q20" s="257"/>
-      <c r="R20" s="257"/>
-      <c r="S20" s="257"/>
-      <c r="T20" s="257"/>
-      <c r="U20" s="257"/>
-      <c r="V20" s="257"/>
+      <c r="L20" s="264"/>
+      <c r="M20" s="264"/>
+      <c r="N20" s="264"/>
+      <c r="O20" s="264"/>
+      <c r="P20" s="264"/>
+      <c r="Q20" s="264"/>
+      <c r="R20" s="264"/>
+      <c r="S20" s="264"/>
+      <c r="T20" s="264"/>
+      <c r="U20" s="264"/>
+      <c r="V20" s="264"/>
     </row>
     <row r="21" spans="1:22" ht="30" customHeight="1">
-      <c r="A21" s="275" t="s">
+      <c r="A21" s="272" t="s">
         <v>823</v>
       </c>
-      <c r="B21" s="276"/>
-      <c r="C21" s="276"/>
-      <c r="D21" s="276"/>
-      <c r="E21" s="276"/>
-      <c r="F21" s="276"/>
-      <c r="G21" s="276"/>
-      <c r="H21" s="276"/>
-      <c r="I21" s="276"/>
+      <c r="B21" s="273"/>
+      <c r="C21" s="273"/>
+      <c r="D21" s="273"/>
+      <c r="E21" s="273"/>
+      <c r="F21" s="273"/>
+      <c r="G21" s="273"/>
+      <c r="H21" s="273"/>
+      <c r="I21" s="273"/>
       <c r="J21">
         <v>12</v>
       </c>
     </row>
     <row r="22" spans="1:22">
-      <c r="A22" s="273" t="s">
+      <c r="A22" s="270" t="s">
         <v>824</v>
       </c>
-      <c r="B22" s="274"/>
-      <c r="C22" s="274"/>
-      <c r="D22" s="274"/>
-      <c r="E22" s="274"/>
-      <c r="F22" s="274"/>
-      <c r="G22" s="274"/>
-      <c r="H22" s="274"/>
-      <c r="I22" s="274"/>
+      <c r="B22" s="271"/>
+      <c r="C22" s="271"/>
+      <c r="D22" s="271"/>
+      <c r="E22" s="271"/>
+      <c r="F22" s="271"/>
+      <c r="G22" s="271"/>
+      <c r="H22" s="271"/>
+      <c r="I22" s="271"/>
       <c r="J22">
         <v>12</v>
       </c>
     </row>
     <row r="23" spans="1:22" ht="30.75" customHeight="1">
-      <c r="A23" s="263" t="s">
+      <c r="A23" s="274" t="s">
         <v>237</v>
       </c>
-      <c r="B23" s="264"/>
-      <c r="C23" s="264"/>
-      <c r="D23" s="264"/>
-      <c r="E23" s="264"/>
-      <c r="F23" s="264"/>
-      <c r="G23" s="264"/>
-      <c r="H23" s="264"/>
-      <c r="I23" s="264"/>
+      <c r="B23" s="275"/>
+      <c r="C23" s="275"/>
+      <c r="D23" s="275"/>
+      <c r="E23" s="275"/>
+      <c r="F23" s="275"/>
+      <c r="G23" s="275"/>
+      <c r="H23" s="275"/>
+      <c r="I23" s="275"/>
       <c r="J23">
         <v>13</v>
       </c>
     </row>
     <row r="24" spans="1:22">
-      <c r="A24" s="257" t="s">
+      <c r="A24" s="264" t="s">
         <v>826</v>
       </c>
-      <c r="B24" s="257"/>
-      <c r="C24" s="257"/>
-      <c r="D24" s="257"/>
-      <c r="E24" s="257"/>
-      <c r="F24" s="257"/>
-      <c r="G24" s="257"/>
-      <c r="H24" s="257"/>
-      <c r="I24" s="257"/>
+      <c r="B24" s="264"/>
+      <c r="C24" s="264"/>
+      <c r="D24" s="264"/>
+      <c r="E24" s="264"/>
+      <c r="F24" s="264"/>
+      <c r="G24" s="264"/>
+      <c r="H24" s="264"/>
+      <c r="I24" s="264"/>
       <c r="J24">
         <v>14</v>
       </c>
     </row>
     <row r="25" spans="1:22">
-      <c r="A25" s="272" t="s">
+      <c r="A25" s="279" t="s">
         <v>827</v>
       </c>
-      <c r="B25" s="272"/>
-      <c r="C25" s="272"/>
-      <c r="D25" s="272"/>
-      <c r="E25" s="272"/>
-      <c r="F25" s="272"/>
-      <c r="G25" s="272"/>
-      <c r="H25" s="272"/>
-      <c r="I25" s="272"/>
+      <c r="B25" s="279"/>
+      <c r="C25" s="279"/>
+      <c r="D25" s="279"/>
+      <c r="E25" s="279"/>
+      <c r="F25" s="279"/>
+      <c r="G25" s="279"/>
+      <c r="H25" s="279"/>
+      <c r="I25" s="279"/>
       <c r="J25">
         <v>14</v>
       </c>
     </row>
     <row r="26" spans="1:22" ht="30.75" customHeight="1">
-      <c r="A26" s="258" t="s">
+      <c r="A26" s="276" t="s">
         <v>828</v>
       </c>
-      <c r="B26" s="258"/>
-      <c r="C26" s="258"/>
-      <c r="D26" s="258"/>
-      <c r="E26" s="258"/>
-      <c r="F26" s="258"/>
-      <c r="G26" s="258"/>
-      <c r="H26" s="258"/>
-      <c r="I26" s="258"/>
+      <c r="B26" s="276"/>
+      <c r="C26" s="276"/>
+      <c r="D26" s="276"/>
+      <c r="E26" s="276"/>
+      <c r="F26" s="276"/>
+      <c r="G26" s="276"/>
+      <c r="H26" s="276"/>
+      <c r="I26" s="276"/>
       <c r="J26">
         <v>14</v>
       </c>
     </row>
     <row r="27" spans="1:22">
-      <c r="A27" s="265" t="s">
+      <c r="A27" s="257" t="s">
         <v>829</v>
       </c>
-      <c r="B27" s="265"/>
-      <c r="C27" s="265"/>
-      <c r="D27" s="265"/>
-      <c r="E27" s="265"/>
-      <c r="F27" s="265"/>
-      <c r="G27" s="265"/>
-      <c r="H27" s="265"/>
-      <c r="I27" s="265"/>
+      <c r="B27" s="257"/>
+      <c r="C27" s="257"/>
+      <c r="D27" s="257"/>
+      <c r="E27" s="257"/>
+      <c r="F27" s="257"/>
+      <c r="G27" s="257"/>
+      <c r="H27" s="257"/>
+      <c r="I27" s="257"/>
       <c r="J27">
         <v>16</v>
       </c>
     </row>
     <row r="28" spans="1:22">
-      <c r="A28" s="259" t="s">
+      <c r="A28" s="260" t="s">
         <v>830</v>
       </c>
-      <c r="B28" s="260"/>
-      <c r="C28" s="260"/>
-      <c r="D28" s="260"/>
-      <c r="E28" s="260"/>
-      <c r="F28" s="260"/>
-      <c r="G28" s="260"/>
-      <c r="H28" s="260"/>
-      <c r="I28" s="260"/>
+      <c r="B28" s="261"/>
+      <c r="C28" s="261"/>
+      <c r="D28" s="261"/>
+      <c r="E28" s="261"/>
+      <c r="F28" s="261"/>
+      <c r="G28" s="261"/>
+      <c r="H28" s="261"/>
+      <c r="I28" s="261"/>
       <c r="J28">
         <v>17</v>
       </c>
     </row>
     <row r="29" spans="1:22">
-      <c r="A29" s="268" t="s">
+      <c r="A29" s="277" t="s">
         <v>831</v>
       </c>
-      <c r="B29" s="269"/>
-      <c r="C29" s="269"/>
-      <c r="D29" s="269"/>
-      <c r="E29" s="269"/>
-      <c r="F29" s="269"/>
-      <c r="G29" s="269"/>
-      <c r="H29" s="269"/>
-      <c r="I29" s="269"/>
+      <c r="B29" s="278"/>
+      <c r="C29" s="278"/>
+      <c r="D29" s="278"/>
+      <c r="E29" s="278"/>
+      <c r="F29" s="278"/>
+      <c r="G29" s="278"/>
+      <c r="H29" s="278"/>
+      <c r="I29" s="278"/>
       <c r="J29">
         <v>19</v>
       </c>
     </row>
     <row r="30" spans="1:22" ht="30.75" customHeight="1">
-      <c r="A30" s="263" t="s">
+      <c r="A30" s="274" t="s">
         <v>832</v>
       </c>
-      <c r="B30" s="264"/>
-      <c r="C30" s="264"/>
-      <c r="D30" s="264"/>
-      <c r="E30" s="264"/>
-      <c r="F30" s="264"/>
-      <c r="G30" s="264"/>
-      <c r="H30" s="264"/>
-      <c r="I30" s="264"/>
+      <c r="B30" s="275"/>
+      <c r="C30" s="275"/>
+      <c r="D30" s="275"/>
+      <c r="E30" s="275"/>
+      <c r="F30" s="275"/>
+      <c r="G30" s="275"/>
+      <c r="H30" s="275"/>
+      <c r="I30" s="275"/>
       <c r="J30">
         <v>21</v>
       </c>
     </row>
     <row r="31" spans="1:22" ht="30" customHeight="1">
-      <c r="A31" s="256" t="s">
+      <c r="A31" s="280" t="s">
         <v>834</v>
       </c>
-      <c r="B31" s="256"/>
-      <c r="C31" s="256"/>
-      <c r="D31" s="256"/>
-      <c r="E31" s="256"/>
-      <c r="F31" s="256"/>
-      <c r="G31" s="256"/>
-      <c r="H31" s="256"/>
-      <c r="I31" s="256"/>
+      <c r="B31" s="280"/>
+      <c r="C31" s="280"/>
+      <c r="D31" s="280"/>
+      <c r="E31" s="280"/>
+      <c r="F31" s="280"/>
+      <c r="G31" s="280"/>
+      <c r="H31" s="280"/>
+      <c r="I31" s="280"/>
       <c r="J31">
         <v>21</v>
       </c>
     </row>
     <row r="32" spans="1:22">
-      <c r="A32" s="257" t="s">
+      <c r="A32" s="264" t="s">
         <v>835</v>
       </c>
-      <c r="B32" s="257"/>
-      <c r="C32" s="257"/>
-      <c r="D32" s="257"/>
-      <c r="E32" s="257"/>
-      <c r="F32" s="257"/>
-      <c r="G32" s="257"/>
-      <c r="H32" s="257"/>
-      <c r="I32" s="257"/>
+      <c r="B32" s="264"/>
+      <c r="C32" s="264"/>
+      <c r="D32" s="264"/>
+      <c r="E32" s="264"/>
+      <c r="F32" s="264"/>
+      <c r="G32" s="264"/>
+      <c r="H32" s="264"/>
+      <c r="I32" s="264"/>
       <c r="J32">
         <v>21</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="29.25" customHeight="1">
-      <c r="A33" s="270" t="s">
+      <c r="A33" s="281" t="s">
         <v>836</v>
       </c>
-      <c r="B33" s="270"/>
-      <c r="C33" s="270"/>
-      <c r="D33" s="270"/>
-      <c r="E33" s="270"/>
-      <c r="F33" s="270"/>
-      <c r="G33" s="270"/>
-      <c r="H33" s="270"/>
-      <c r="I33" s="270"/>
+      <c r="B33" s="281"/>
+      <c r="C33" s="281"/>
+      <c r="D33" s="281"/>
+      <c r="E33" s="281"/>
+      <c r="F33" s="281"/>
+      <c r="G33" s="281"/>
+      <c r="H33" s="281"/>
+      <c r="I33" s="281"/>
       <c r="J33">
         <v>22</v>
       </c>
     </row>
     <row r="34" spans="1:10">
-      <c r="A34" s="271" t="s">
+      <c r="A34" s="282" t="s">
         <v>837</v>
       </c>
-      <c r="B34" s="271"/>
-      <c r="C34" s="271"/>
-      <c r="D34" s="271"/>
-      <c r="E34" s="271"/>
-      <c r="F34" s="271"/>
-      <c r="G34" s="271"/>
-      <c r="H34" s="271"/>
-      <c r="I34" s="271"/>
+      <c r="B34" s="282"/>
+      <c r="C34" s="282"/>
+      <c r="D34" s="282"/>
+      <c r="E34" s="282"/>
+      <c r="F34" s="282"/>
+      <c r="G34" s="282"/>
+      <c r="H34" s="282"/>
+      <c r="I34" s="282"/>
       <c r="J34">
         <v>25</v>
       </c>
     </row>
     <row r="35" spans="1:10">
-      <c r="A35" s="272" t="s">
+      <c r="A35" s="279" t="s">
         <v>838</v>
       </c>
-      <c r="B35" s="272"/>
-      <c r="C35" s="272"/>
-      <c r="D35" s="272"/>
-      <c r="E35" s="272"/>
-      <c r="F35" s="272"/>
-      <c r="G35" s="272"/>
-      <c r="H35" s="272"/>
-      <c r="I35" s="272"/>
+      <c r="B35" s="279"/>
+      <c r="C35" s="279"/>
+      <c r="D35" s="279"/>
+      <c r="E35" s="279"/>
+      <c r="F35" s="279"/>
+      <c r="G35" s="279"/>
+      <c r="H35" s="279"/>
+      <c r="I35" s="279"/>
       <c r="J35">
         <v>25</v>
       </c>
     </row>
     <row r="36" spans="1:10">
-      <c r="A36" s="259" t="s">
+      <c r="A36" s="260" t="s">
         <v>839</v>
       </c>
-      <c r="B36" s="260"/>
-      <c r="C36" s="260"/>
-      <c r="D36" s="260"/>
-      <c r="E36" s="260"/>
-      <c r="F36" s="260"/>
-      <c r="G36" s="260"/>
-      <c r="H36" s="260"/>
-      <c r="I36" s="260"/>
+      <c r="B36" s="261"/>
+      <c r="C36" s="261"/>
+      <c r="D36" s="261"/>
+      <c r="E36" s="261"/>
+      <c r="F36" s="261"/>
+      <c r="G36" s="261"/>
+      <c r="H36" s="261"/>
+      <c r="I36" s="261"/>
       <c r="J36">
         <v>25</v>
       </c>
     </row>
     <row r="37" spans="1:10">
-      <c r="A37" s="261" t="s">
+      <c r="A37" s="266" t="s">
         <v>840</v>
       </c>
-      <c r="B37" s="262"/>
-      <c r="C37" s="262"/>
-      <c r="D37" s="262"/>
-      <c r="E37" s="262"/>
-      <c r="F37" s="262"/>
-      <c r="G37" s="262"/>
-      <c r="H37" s="262"/>
-      <c r="I37" s="262"/>
+      <c r="B37" s="267"/>
+      <c r="C37" s="267"/>
+      <c r="D37" s="267"/>
+      <c r="E37" s="267"/>
+      <c r="F37" s="267"/>
+      <c r="G37" s="267"/>
+      <c r="H37" s="267"/>
+      <c r="I37" s="267"/>
       <c r="J37">
         <v>25</v>
       </c>
     </row>
     <row r="38" spans="1:10">
-      <c r="A38" s="261" t="s">
+      <c r="A38" s="266" t="s">
         <v>841</v>
       </c>
-      <c r="B38" s="262"/>
-      <c r="C38" s="262"/>
-      <c r="D38" s="262"/>
-      <c r="E38" s="262"/>
-      <c r="F38" s="262"/>
-      <c r="G38" s="262"/>
-      <c r="H38" s="262"/>
-      <c r="I38" s="262"/>
+      <c r="B38" s="267"/>
+      <c r="C38" s="267"/>
+      <c r="D38" s="267"/>
+      <c r="E38" s="267"/>
+      <c r="F38" s="267"/>
+      <c r="G38" s="267"/>
+      <c r="H38" s="267"/>
+      <c r="I38" s="267"/>
       <c r="J38">
         <v>26</v>
       </c>
     </row>
     <row r="39" spans="1:10">
-      <c r="A39" s="265" t="s">
+      <c r="A39" s="257" t="s">
         <v>842</v>
       </c>
-      <c r="B39" s="265"/>
-      <c r="C39" s="265"/>
-      <c r="D39" s="265"/>
-      <c r="E39" s="265"/>
-      <c r="F39" s="265"/>
-      <c r="G39" s="265"/>
-      <c r="H39" s="265"/>
-      <c r="I39" s="265"/>
+      <c r="B39" s="257"/>
+      <c r="C39" s="257"/>
+      <c r="D39" s="257"/>
+      <c r="E39" s="257"/>
+      <c r="F39" s="257"/>
+      <c r="G39" s="257"/>
+      <c r="H39" s="257"/>
+      <c r="I39" s="257"/>
       <c r="J39">
         <v>26</v>
       </c>
     </row>
     <row r="40" spans="1:10" ht="29.25" customHeight="1">
-      <c r="A40" s="266" t="s">
+      <c r="A40" s="283" t="s">
         <v>843</v>
       </c>
-      <c r="B40" s="267"/>
-      <c r="C40" s="267"/>
-      <c r="D40" s="267"/>
-      <c r="E40" s="267"/>
-      <c r="F40" s="267"/>
-      <c r="G40" s="267"/>
-      <c r="H40" s="267"/>
-      <c r="I40" s="267"/>
+      <c r="B40" s="284"/>
+      <c r="C40" s="284"/>
+      <c r="D40" s="284"/>
+      <c r="E40" s="284"/>
+      <c r="F40" s="284"/>
+      <c r="G40" s="284"/>
+      <c r="H40" s="284"/>
+      <c r="I40" s="284"/>
       <c r="J40">
         <v>29</v>
       </c>
     </row>
     <row r="41" spans="1:10">
-      <c r="A41" s="261" t="s">
+      <c r="A41" s="266" t="s">
         <v>844</v>
       </c>
-      <c r="B41" s="262"/>
-      <c r="C41" s="262"/>
-      <c r="D41" s="262"/>
-      <c r="E41" s="262"/>
-      <c r="F41" s="262"/>
-      <c r="G41" s="262"/>
-      <c r="H41" s="262"/>
-      <c r="I41" s="262"/>
+      <c r="B41" s="267"/>
+      <c r="C41" s="267"/>
+      <c r="D41" s="267"/>
+      <c r="E41" s="267"/>
+      <c r="F41" s="267"/>
+      <c r="G41" s="267"/>
+      <c r="H41" s="267"/>
+      <c r="I41" s="267"/>
       <c r="J41">
         <v>29</v>
       </c>
     </row>
     <row r="42" spans="1:10" ht="30.75" customHeight="1">
-      <c r="A42" s="256" t="s">
+      <c r="A42" s="280" t="s">
         <v>845</v>
       </c>
-      <c r="B42" s="256"/>
-      <c r="C42" s="256"/>
-      <c r="D42" s="256"/>
-      <c r="E42" s="256"/>
-      <c r="F42" s="256"/>
-      <c r="G42" s="256"/>
-      <c r="H42" s="256"/>
-      <c r="I42" s="256"/>
+      <c r="B42" s="280"/>
+      <c r="C42" s="280"/>
+      <c r="D42" s="280"/>
+      <c r="E42" s="280"/>
+      <c r="F42" s="280"/>
+      <c r="G42" s="280"/>
+      <c r="H42" s="280"/>
+      <c r="I42" s="280"/>
       <c r="J42">
         <v>31</v>
       </c>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="257" t="s">
+      <c r="A43" s="264" t="s">
         <v>846</v>
       </c>
-      <c r="B43" s="257"/>
-      <c r="C43" s="257"/>
-      <c r="D43" s="257"/>
-      <c r="E43" s="257"/>
-      <c r="F43" s="257"/>
-      <c r="G43" s="257"/>
-      <c r="H43" s="257"/>
-      <c r="I43" s="257"/>
+      <c r="B43" s="264"/>
+      <c r="C43" s="264"/>
+      <c r="D43" s="264"/>
+      <c r="E43" s="264"/>
+      <c r="F43" s="264"/>
+      <c r="G43" s="264"/>
+      <c r="H43" s="264"/>
+      <c r="I43" s="264"/>
       <c r="J43">
         <v>32</v>
       </c>
     </row>
     <row r="44" spans="1:10" ht="29.25" customHeight="1">
-      <c r="A44" s="256" t="s">
+      <c r="A44" s="280" t="s">
         <v>847</v>
       </c>
-      <c r="B44" s="256"/>
-      <c r="C44" s="256"/>
-      <c r="D44" s="256"/>
-      <c r="E44" s="256"/>
-      <c r="F44" s="256"/>
-      <c r="G44" s="256"/>
-      <c r="H44" s="256"/>
-      <c r="I44" s="256"/>
+      <c r="B44" s="280"/>
+      <c r="C44" s="280"/>
+      <c r="D44" s="280"/>
+      <c r="E44" s="280"/>
+      <c r="F44" s="280"/>
+      <c r="G44" s="280"/>
+      <c r="H44" s="280"/>
+      <c r="I44" s="280"/>
       <c r="J44">
         <v>36</v>
       </c>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="259" t="s">
+      <c r="A45" s="260" t="s">
         <v>848</v>
       </c>
-      <c r="B45" s="260"/>
-      <c r="C45" s="260"/>
-      <c r="D45" s="260"/>
-      <c r="E45" s="260"/>
-      <c r="F45" s="260"/>
-      <c r="G45" s="260"/>
-      <c r="H45" s="260"/>
-      <c r="I45" s="260"/>
+      <c r="B45" s="261"/>
+      <c r="C45" s="261"/>
+      <c r="D45" s="261"/>
+      <c r="E45" s="261"/>
+      <c r="F45" s="261"/>
+      <c r="G45" s="261"/>
+      <c r="H45" s="261"/>
+      <c r="I45" s="261"/>
       <c r="J45">
         <v>38</v>
       </c>
     </row>
     <row r="46" spans="1:10">
-      <c r="A46" s="259" t="s">
+      <c r="A46" s="260" t="s">
         <v>849</v>
       </c>
-      <c r="B46" s="260"/>
-      <c r="C46" s="260"/>
-      <c r="D46" s="260"/>
-      <c r="E46" s="260"/>
-      <c r="F46" s="260"/>
-      <c r="G46" s="260"/>
-      <c r="H46" s="260"/>
-      <c r="I46" s="260"/>
+      <c r="B46" s="261"/>
+      <c r="C46" s="261"/>
+      <c r="D46" s="261"/>
+      <c r="E46" s="261"/>
+      <c r="F46" s="261"/>
+      <c r="G46" s="261"/>
+      <c r="H46" s="261"/>
+      <c r="I46" s="261"/>
       <c r="J46">
         <v>41</v>
       </c>
     </row>
     <row r="47" spans="1:10">
-      <c r="A47" s="261" t="s">
+      <c r="A47" s="266" t="s">
         <v>850</v>
       </c>
-      <c r="B47" s="262"/>
-      <c r="C47" s="262"/>
-      <c r="D47" s="262"/>
-      <c r="E47" s="262"/>
-      <c r="F47" s="262"/>
-      <c r="G47" s="262"/>
-      <c r="H47" s="262"/>
-      <c r="I47" s="262"/>
+      <c r="B47" s="267"/>
+      <c r="C47" s="267"/>
+      <c r="D47" s="267"/>
+      <c r="E47" s="267"/>
+      <c r="F47" s="267"/>
+      <c r="G47" s="267"/>
+      <c r="H47" s="267"/>
+      <c r="I47" s="267"/>
       <c r="J47">
         <v>41</v>
       </c>
     </row>
     <row r="48" spans="1:10">
-      <c r="A48" s="261" t="s">
+      <c r="A48" s="266" t="s">
         <v>851</v>
       </c>
-      <c r="B48" s="262"/>
-      <c r="C48" s="262"/>
-      <c r="D48" s="262"/>
-      <c r="E48" s="262"/>
-      <c r="F48" s="262"/>
-      <c r="G48" s="262"/>
-      <c r="H48" s="262"/>
-      <c r="I48" s="262"/>
+      <c r="B48" s="267"/>
+      <c r="C48" s="267"/>
+      <c r="D48" s="267"/>
+      <c r="E48" s="267"/>
+      <c r="F48" s="267"/>
+      <c r="G48" s="267"/>
+      <c r="H48" s="267"/>
+      <c r="I48" s="267"/>
       <c r="J48">
         <v>41</v>
       </c>
     </row>
     <row r="49" spans="1:10">
-      <c r="A49" s="259" t="s">
+      <c r="A49" s="260" t="s">
         <v>852</v>
       </c>
-      <c r="B49" s="260"/>
-      <c r="C49" s="260"/>
-      <c r="D49" s="260"/>
-      <c r="E49" s="260"/>
-      <c r="F49" s="260"/>
-      <c r="G49" s="260"/>
-      <c r="H49" s="260"/>
-      <c r="I49" s="260"/>
+      <c r="B49" s="261"/>
+      <c r="C49" s="261"/>
+      <c r="D49" s="261"/>
+      <c r="E49" s="261"/>
+      <c r="F49" s="261"/>
+      <c r="G49" s="261"/>
+      <c r="H49" s="261"/>
+      <c r="I49" s="261"/>
       <c r="J49">
         <v>41</v>
       </c>
     </row>
     <row r="50" spans="1:10" ht="27.75" customHeight="1">
-      <c r="A50" s="258" t="s">
+      <c r="A50" s="276" t="s">
         <v>853</v>
       </c>
-      <c r="B50" s="258"/>
-      <c r="C50" s="258"/>
-      <c r="D50" s="258"/>
-      <c r="E50" s="258"/>
-      <c r="F50" s="258"/>
-      <c r="G50" s="258"/>
-      <c r="H50" s="258"/>
-      <c r="I50" s="258"/>
+      <c r="B50" s="276"/>
+      <c r="C50" s="276"/>
+      <c r="D50" s="276"/>
+      <c r="E50" s="276"/>
+      <c r="F50" s="276"/>
+      <c r="G50" s="276"/>
+      <c r="H50" s="276"/>
+      <c r="I50" s="276"/>
       <c r="J50">
         <v>42</v>
       </c>
     </row>
     <row r="51" spans="1:10">
-      <c r="A51" s="259" t="s">
+      <c r="A51" s="260" t="s">
         <v>854</v>
       </c>
-      <c r="B51" s="260"/>
-      <c r="C51" s="260"/>
-      <c r="D51" s="260"/>
-      <c r="E51" s="260"/>
-      <c r="F51" s="260"/>
-      <c r="G51" s="260"/>
-      <c r="H51" s="260"/>
-      <c r="I51" s="260"/>
+      <c r="B51" s="261"/>
+      <c r="C51" s="261"/>
+      <c r="D51" s="261"/>
+      <c r="E51" s="261"/>
+      <c r="F51" s="261"/>
+      <c r="G51" s="261"/>
+      <c r="H51" s="261"/>
+      <c r="I51" s="261"/>
       <c r="J51">
         <v>43</v>
       </c>
     </row>
     <row r="52" spans="1:10" ht="30" customHeight="1">
-      <c r="A52" s="258" t="s">
+      <c r="A52" s="276" t="s">
         <v>855</v>
       </c>
-      <c r="B52" s="258"/>
-      <c r="C52" s="258"/>
-      <c r="D52" s="258"/>
-      <c r="E52" s="258"/>
-      <c r="F52" s="258"/>
-      <c r="G52" s="258"/>
-      <c r="H52" s="258"/>
-      <c r="I52" s="258"/>
+      <c r="B52" s="276"/>
+      <c r="C52" s="276"/>
+      <c r="D52" s="276"/>
+      <c r="E52" s="276"/>
+      <c r="F52" s="276"/>
+      <c r="G52" s="276"/>
+      <c r="H52" s="276"/>
+      <c r="I52" s="276"/>
       <c r="J52">
         <v>43</v>
       </c>
     </row>
     <row r="53" spans="1:10">
-      <c r="A53" s="257" t="s">
+      <c r="A53" s="264" t="s">
         <v>856</v>
       </c>
-      <c r="B53" s="257"/>
-      <c r="C53" s="257"/>
-      <c r="D53" s="257"/>
-      <c r="E53" s="257"/>
-      <c r="F53" s="257"/>
-      <c r="G53" s="257"/>
-      <c r="H53" s="257"/>
-      <c r="I53" s="257"/>
+      <c r="B53" s="264"/>
+      <c r="C53" s="264"/>
+      <c r="D53" s="264"/>
+      <c r="E53" s="264"/>
+      <c r="F53" s="264"/>
+      <c r="G53" s="264"/>
+      <c r="H53" s="264"/>
+      <c r="I53" s="264"/>
       <c r="J53">
         <v>44</v>
       </c>
     </row>
     <row r="54" spans="1:10">
-      <c r="A54" s="261" t="s">
+      <c r="A54" s="266" t="s">
         <v>857</v>
       </c>
-      <c r="B54" s="262"/>
-      <c r="C54" s="262"/>
-      <c r="D54" s="262"/>
-      <c r="E54" s="262"/>
-      <c r="F54" s="262"/>
-      <c r="G54" s="262"/>
-      <c r="H54" s="262"/>
-      <c r="I54" s="262"/>
+      <c r="B54" s="267"/>
+      <c r="C54" s="267"/>
+      <c r="D54" s="267"/>
+      <c r="E54" s="267"/>
+      <c r="F54" s="267"/>
+      <c r="G54" s="267"/>
+      <c r="H54" s="267"/>
+      <c r="I54" s="267"/>
       <c r="J54">
         <v>44</v>
       </c>
     </row>
     <row r="55" spans="1:10" ht="30" customHeight="1">
-      <c r="A55" s="263" t="s">
+      <c r="A55" s="274" t="s">
         <v>858</v>
       </c>
-      <c r="B55" s="264"/>
-      <c r="C55" s="264"/>
-      <c r="D55" s="264"/>
-      <c r="E55" s="264"/>
-      <c r="F55" s="264"/>
-      <c r="G55" s="264"/>
-      <c r="H55" s="264"/>
-      <c r="I55" s="264"/>
+      <c r="B55" s="275"/>
+      <c r="C55" s="275"/>
+      <c r="D55" s="275"/>
+      <c r="E55" s="275"/>
+      <c r="F55" s="275"/>
+      <c r="G55" s="275"/>
+      <c r="H55" s="275"/>
+      <c r="I55" s="275"/>
       <c r="J55" s="210" t="s">
         <v>860</v>
       </c>
     </row>
     <row r="56" spans="1:10" ht="30.75" customHeight="1">
-      <c r="A56" s="256" t="s">
+      <c r="A56" s="280" t="s">
         <v>859</v>
       </c>
-      <c r="B56" s="256"/>
-      <c r="C56" s="256"/>
-      <c r="D56" s="256"/>
-      <c r="E56" s="256"/>
-      <c r="F56" s="256"/>
-      <c r="G56" s="256"/>
-      <c r="H56" s="256"/>
-      <c r="I56" s="256"/>
+      <c r="B56" s="280"/>
+      <c r="C56" s="280"/>
+      <c r="D56" s="280"/>
+      <c r="E56" s="280"/>
+      <c r="F56" s="280"/>
+      <c r="G56" s="280"/>
+      <c r="H56" s="280"/>
+      <c r="I56" s="280"/>
       <c r="J56">
         <v>47</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="56">
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A13:I13"/>
-    <mergeCell ref="A2:I2"/>
-    <mergeCell ref="A3:I3"/>
-    <mergeCell ref="A4:I4"/>
-    <mergeCell ref="A5:I5"/>
-    <mergeCell ref="A6:I6"/>
-    <mergeCell ref="A7:I7"/>
-    <mergeCell ref="A8:I8"/>
-    <mergeCell ref="A9:I9"/>
-    <mergeCell ref="A10:I10"/>
-    <mergeCell ref="A11:I11"/>
-    <mergeCell ref="A12:I12"/>
-    <mergeCell ref="A14:I14"/>
-    <mergeCell ref="A15:I15"/>
-    <mergeCell ref="A16:I16"/>
-    <mergeCell ref="A17:I17"/>
-    <mergeCell ref="K20:V20"/>
-    <mergeCell ref="A22:I22"/>
-    <mergeCell ref="A18:I18"/>
-    <mergeCell ref="A23:I23"/>
-    <mergeCell ref="A26:I26"/>
-    <mergeCell ref="A19:I19"/>
-    <mergeCell ref="A24:I24"/>
-    <mergeCell ref="A25:I25"/>
-    <mergeCell ref="A21:I21"/>
-    <mergeCell ref="A37:I37"/>
-    <mergeCell ref="A27:I27"/>
-    <mergeCell ref="A28:I28"/>
-    <mergeCell ref="A29:I29"/>
-    <mergeCell ref="A30:I30"/>
-    <mergeCell ref="A31:I31"/>
-    <mergeCell ref="A32:I32"/>
-    <mergeCell ref="A33:I33"/>
-    <mergeCell ref="A34:I34"/>
-    <mergeCell ref="A35:I35"/>
-    <mergeCell ref="A36:I36"/>
-    <mergeCell ref="A38:I38"/>
-    <mergeCell ref="A39:I39"/>
-    <mergeCell ref="A40:I40"/>
-    <mergeCell ref="A41:I41"/>
-    <mergeCell ref="A42:I42"/>
     <mergeCell ref="A56:I56"/>
     <mergeCell ref="A43:I43"/>
     <mergeCell ref="A52:I52"/>
@@ -16245,6 +16359,48 @@
     <mergeCell ref="A49:I49"/>
     <mergeCell ref="A50:I50"/>
     <mergeCell ref="A44:I44"/>
+    <mergeCell ref="A38:I38"/>
+    <mergeCell ref="A39:I39"/>
+    <mergeCell ref="A40:I40"/>
+    <mergeCell ref="A41:I41"/>
+    <mergeCell ref="A42:I42"/>
+    <mergeCell ref="A37:I37"/>
+    <mergeCell ref="A27:I27"/>
+    <mergeCell ref="A28:I28"/>
+    <mergeCell ref="A29:I29"/>
+    <mergeCell ref="A30:I30"/>
+    <mergeCell ref="A31:I31"/>
+    <mergeCell ref="A32:I32"/>
+    <mergeCell ref="A33:I33"/>
+    <mergeCell ref="A34:I34"/>
+    <mergeCell ref="A35:I35"/>
+    <mergeCell ref="A36:I36"/>
+    <mergeCell ref="A22:I22"/>
+    <mergeCell ref="A18:I18"/>
+    <mergeCell ref="A23:I23"/>
+    <mergeCell ref="A26:I26"/>
+    <mergeCell ref="A19:I19"/>
+    <mergeCell ref="A24:I24"/>
+    <mergeCell ref="A25:I25"/>
+    <mergeCell ref="A21:I21"/>
+    <mergeCell ref="A14:I14"/>
+    <mergeCell ref="A15:I15"/>
+    <mergeCell ref="A16:I16"/>
+    <mergeCell ref="A17:I17"/>
+    <mergeCell ref="K20:V20"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A13:I13"/>
+    <mergeCell ref="A2:I2"/>
+    <mergeCell ref="A3:I3"/>
+    <mergeCell ref="A4:I4"/>
+    <mergeCell ref="A5:I5"/>
+    <mergeCell ref="A6:I6"/>
+    <mergeCell ref="A7:I7"/>
+    <mergeCell ref="A8:I8"/>
+    <mergeCell ref="A9:I9"/>
+    <mergeCell ref="A10:I10"/>
+    <mergeCell ref="A11:I11"/>
+    <mergeCell ref="A12:I12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -16873,43 +17029,43 @@
   <sheetFormatPr defaultRowHeight="14.5"/>
   <sheetData>
     <row r="1" spans="1:24" s="161" customFormat="1">
-      <c r="A1" s="307" t="s">
+      <c r="A1" s="302" t="s">
         <v>733</v>
       </c>
-      <c r="B1" s="307"/>
-      <c r="C1" s="307"/>
-      <c r="D1" s="307"/>
-      <c r="E1" s="307"/>
-      <c r="F1" s="307"/>
-      <c r="G1" s="307"/>
-      <c r="H1" s="307"/>
-      <c r="I1" s="307"/>
-      <c r="J1" s="307"/>
-      <c r="K1" s="307"/>
-      <c r="L1" s="307"/>
-      <c r="M1" s="307"/>
-      <c r="N1" s="307"/>
-      <c r="O1" s="307"/>
-      <c r="P1" s="307"/>
-      <c r="Q1" s="307"/>
-      <c r="R1" s="307"/>
-      <c r="S1" s="307"/>
-      <c r="T1" s="307"/>
-      <c r="U1" s="307"/>
-      <c r="V1" s="307"/>
-      <c r="W1" s="307"/>
-      <c r="X1" s="307"/>
+      <c r="B1" s="302"/>
+      <c r="C1" s="302"/>
+      <c r="D1" s="302"/>
+      <c r="E1" s="302"/>
+      <c r="F1" s="302"/>
+      <c r="G1" s="302"/>
+      <c r="H1" s="302"/>
+      <c r="I1" s="302"/>
+      <c r="J1" s="302"/>
+      <c r="K1" s="302"/>
+      <c r="L1" s="302"/>
+      <c r="M1" s="302"/>
+      <c r="N1" s="302"/>
+      <c r="O1" s="302"/>
+      <c r="P1" s="302"/>
+      <c r="Q1" s="302"/>
+      <c r="R1" s="302"/>
+      <c r="S1" s="302"/>
+      <c r="T1" s="302"/>
+      <c r="U1" s="302"/>
+      <c r="V1" s="302"/>
+      <c r="W1" s="302"/>
+      <c r="X1" s="302"/>
     </row>
     <row r="2" spans="1:24">
-      <c r="A2" s="302" t="s">
+      <c r="A2" s="311" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="302"/>
-      <c r="C2" s="302"/>
-      <c r="D2" s="302"/>
-      <c r="E2" s="302"/>
-      <c r="F2" s="302"/>
-      <c r="G2" s="302"/>
+      <c r="B2" s="311"/>
+      <c r="C2" s="311"/>
+      <c r="D2" s="311"/>
+      <c r="E2" s="311"/>
+      <c r="F2" s="311"/>
+      <c r="G2" s="311"/>
       <c r="H2" s="251" t="s">
         <v>734</v>
       </c>
@@ -16931,15 +17087,15 @@
       <c r="X2" s="251"/>
     </row>
     <row r="3" spans="1:24">
-      <c r="A3" s="302" t="s">
+      <c r="A3" s="311" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="302"/>
-      <c r="C3" s="302"/>
-      <c r="D3" s="302"/>
-      <c r="E3" s="302"/>
-      <c r="F3" s="302"/>
-      <c r="G3" s="302"/>
+      <c r="B3" s="311"/>
+      <c r="C3" s="311"/>
+      <c r="D3" s="311"/>
+      <c r="E3" s="311"/>
+      <c r="F3" s="311"/>
+      <c r="G3" s="311"/>
       <c r="H3" s="251" t="s">
         <v>735</v>
       </c>
@@ -16961,32 +17117,32 @@
       <c r="X3" s="251"/>
     </row>
     <row r="4" spans="1:24">
-      <c r="A4" s="308" t="s">
+      <c r="A4" s="303" t="s">
         <v>736</v>
       </c>
-      <c r="B4" s="308"/>
-      <c r="C4" s="308"/>
-      <c r="D4" s="308"/>
-      <c r="E4" s="308"/>
-      <c r="F4" s="308"/>
-      <c r="G4" s="308"/>
-      <c r="H4" s="308"/>
-      <c r="I4" s="308"/>
-      <c r="J4" s="308"/>
-      <c r="K4" s="308"/>
-      <c r="L4" s="308"/>
-      <c r="M4" s="308"/>
-      <c r="N4" s="308"/>
-      <c r="O4" s="308"/>
-      <c r="P4" s="308"/>
-      <c r="Q4" s="308"/>
-      <c r="R4" s="308"/>
-      <c r="S4" s="308"/>
-      <c r="T4" s="308"/>
-      <c r="U4" s="308"/>
-      <c r="V4" s="308"/>
-      <c r="W4" s="308"/>
-      <c r="X4" s="308"/>
+      <c r="B4" s="303"/>
+      <c r="C4" s="303"/>
+      <c r="D4" s="303"/>
+      <c r="E4" s="303"/>
+      <c r="F4" s="303"/>
+      <c r="G4" s="303"/>
+      <c r="H4" s="303"/>
+      <c r="I4" s="303"/>
+      <c r="J4" s="303"/>
+      <c r="K4" s="303"/>
+      <c r="L4" s="303"/>
+      <c r="M4" s="303"/>
+      <c r="N4" s="303"/>
+      <c r="O4" s="303"/>
+      <c r="P4" s="303"/>
+      <c r="Q4" s="303"/>
+      <c r="R4" s="303"/>
+      <c r="S4" s="303"/>
+      <c r="T4" s="303"/>
+      <c r="U4" s="303"/>
+      <c r="V4" s="303"/>
+      <c r="W4" s="303"/>
+      <c r="X4" s="303"/>
     </row>
     <row r="5" spans="1:24">
       <c r="A5" s="254" t="s">
@@ -17229,43 +17385,43 @@
       <c r="X12" s="251"/>
     </row>
     <row r="13" spans="1:24">
-      <c r="A13" s="309" t="s">
+      <c r="A13" s="304" t="s">
         <v>746</v>
       </c>
-      <c r="B13" s="309"/>
-      <c r="C13" s="309"/>
-      <c r="D13" s="309"/>
-      <c r="E13" s="309"/>
-      <c r="F13" s="309"/>
-      <c r="G13" s="309"/>
-      <c r="H13" s="309"/>
-      <c r="I13" s="309"/>
-      <c r="J13" s="309"/>
-      <c r="K13" s="309"/>
-      <c r="L13" s="309"/>
-      <c r="M13" s="309"/>
-      <c r="N13" s="309"/>
-      <c r="O13" s="309"/>
-      <c r="P13" s="309"/>
-      <c r="Q13" s="309"/>
-      <c r="R13" s="309"/>
-      <c r="S13" s="309"/>
-      <c r="T13" s="309"/>
-      <c r="U13" s="309"/>
-      <c r="V13" s="309"/>
-      <c r="W13" s="309"/>
-      <c r="X13" s="309"/>
+      <c r="B13" s="304"/>
+      <c r="C13" s="304"/>
+      <c r="D13" s="304"/>
+      <c r="E13" s="304"/>
+      <c r="F13" s="304"/>
+      <c r="G13" s="304"/>
+      <c r="H13" s="304"/>
+      <c r="I13" s="304"/>
+      <c r="J13" s="304"/>
+      <c r="K13" s="304"/>
+      <c r="L13" s="304"/>
+      <c r="M13" s="304"/>
+      <c r="N13" s="304"/>
+      <c r="O13" s="304"/>
+      <c r="P13" s="304"/>
+      <c r="Q13" s="304"/>
+      <c r="R13" s="304"/>
+      <c r="S13" s="304"/>
+      <c r="T13" s="304"/>
+      <c r="U13" s="304"/>
+      <c r="V13" s="304"/>
+      <c r="W13" s="304"/>
+      <c r="X13" s="304"/>
     </row>
     <row r="14" spans="1:24">
-      <c r="A14" s="306" t="s">
+      <c r="A14" s="307" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="306"/>
-      <c r="C14" s="306"/>
-      <c r="D14" s="306"/>
-      <c r="E14" s="306"/>
-      <c r="F14" s="306"/>
-      <c r="G14" s="306"/>
+      <c r="B14" s="307"/>
+      <c r="C14" s="307"/>
+      <c r="D14" s="307"/>
+      <c r="E14" s="307"/>
+      <c r="F14" s="307"/>
+      <c r="G14" s="307"/>
       <c r="H14" s="251" t="s">
         <v>747</v>
       </c>
@@ -17287,15 +17443,15 @@
       <c r="X14" s="251"/>
     </row>
     <row r="15" spans="1:24">
-      <c r="A15" s="306" t="s">
+      <c r="A15" s="307" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="306"/>
-      <c r="C15" s="306"/>
-      <c r="D15" s="306"/>
-      <c r="E15" s="306"/>
-      <c r="F15" s="306"/>
-      <c r="G15" s="306"/>
+      <c r="B15" s="307"/>
+      <c r="C15" s="307"/>
+      <c r="D15" s="307"/>
+      <c r="E15" s="307"/>
+      <c r="F15" s="307"/>
+      <c r="G15" s="307"/>
       <c r="H15" s="251" t="s">
         <v>748</v>
       </c>
@@ -17317,15 +17473,15 @@
       <c r="X15" s="251"/>
     </row>
     <row r="16" spans="1:24">
-      <c r="A16" s="306" t="s">
+      <c r="A16" s="307" t="s">
         <v>749</v>
       </c>
-      <c r="B16" s="306"/>
-      <c r="C16" s="306"/>
-      <c r="D16" s="306"/>
-      <c r="E16" s="306"/>
-      <c r="F16" s="306"/>
-      <c r="G16" s="306"/>
+      <c r="B16" s="307"/>
+      <c r="C16" s="307"/>
+      <c r="D16" s="307"/>
+      <c r="E16" s="307"/>
+      <c r="F16" s="307"/>
+      <c r="G16" s="307"/>
       <c r="H16" s="251" t="s">
         <v>750</v>
       </c>
@@ -17347,15 +17503,15 @@
       <c r="X16" s="251"/>
     </row>
     <row r="17" spans="1:24">
-      <c r="A17" s="306" t="s">
+      <c r="A17" s="307" t="s">
         <v>21</v>
       </c>
-      <c r="B17" s="306"/>
-      <c r="C17" s="306"/>
-      <c r="D17" s="306"/>
-      <c r="E17" s="306"/>
-      <c r="F17" s="306"/>
-      <c r="G17" s="306"/>
+      <c r="B17" s="307"/>
+      <c r="C17" s="307"/>
+      <c r="D17" s="307"/>
+      <c r="E17" s="307"/>
+      <c r="F17" s="307"/>
+      <c r="G17" s="307"/>
       <c r="H17" s="251" t="s">
         <v>751</v>
       </c>
@@ -17377,15 +17533,15 @@
       <c r="X17" s="251"/>
     </row>
     <row r="18" spans="1:24">
-      <c r="A18" s="306" t="s">
+      <c r="A18" s="307" t="s">
         <v>752</v>
       </c>
-      <c r="B18" s="306"/>
-      <c r="C18" s="306"/>
-      <c r="D18" s="306"/>
-      <c r="E18" s="306"/>
-      <c r="F18" s="306"/>
-      <c r="G18" s="306"/>
+      <c r="B18" s="307"/>
+      <c r="C18" s="307"/>
+      <c r="D18" s="307"/>
+      <c r="E18" s="307"/>
+      <c r="F18" s="307"/>
+      <c r="G18" s="307"/>
       <c r="H18" s="251" t="s">
         <v>753</v>
       </c>
@@ -17407,43 +17563,43 @@
       <c r="X18" s="251"/>
     </row>
     <row r="19" spans="1:24">
-      <c r="A19" s="307" t="s">
+      <c r="A19" s="302" t="s">
         <v>754</v>
       </c>
-      <c r="B19" s="307"/>
-      <c r="C19" s="307"/>
-      <c r="D19" s="307"/>
-      <c r="E19" s="307"/>
-      <c r="F19" s="307"/>
-      <c r="G19" s="307"/>
-      <c r="H19" s="307"/>
-      <c r="I19" s="307"/>
-      <c r="J19" s="307"/>
-      <c r="K19" s="307"/>
-      <c r="L19" s="307"/>
-      <c r="M19" s="307"/>
-      <c r="N19" s="307"/>
-      <c r="O19" s="307"/>
-      <c r="P19" s="307"/>
-      <c r="Q19" s="307"/>
-      <c r="R19" s="307"/>
-      <c r="S19" s="307"/>
-      <c r="T19" s="307"/>
-      <c r="U19" s="307"/>
-      <c r="V19" s="307"/>
-      <c r="W19" s="307"/>
-      <c r="X19" s="307"/>
+      <c r="B19" s="302"/>
+      <c r="C19" s="302"/>
+      <c r="D19" s="302"/>
+      <c r="E19" s="302"/>
+      <c r="F19" s="302"/>
+      <c r="G19" s="302"/>
+      <c r="H19" s="302"/>
+      <c r="I19" s="302"/>
+      <c r="J19" s="302"/>
+      <c r="K19" s="302"/>
+      <c r="L19" s="302"/>
+      <c r="M19" s="302"/>
+      <c r="N19" s="302"/>
+      <c r="O19" s="302"/>
+      <c r="P19" s="302"/>
+      <c r="Q19" s="302"/>
+      <c r="R19" s="302"/>
+      <c r="S19" s="302"/>
+      <c r="T19" s="302"/>
+      <c r="U19" s="302"/>
+      <c r="V19" s="302"/>
+      <c r="W19" s="302"/>
+      <c r="X19" s="302"/>
     </row>
     <row r="20" spans="1:24">
-      <c r="A20" s="303" t="s">
+      <c r="A20" s="308" t="s">
         <v>23</v>
       </c>
-      <c r="B20" s="303"/>
-      <c r="C20" s="303"/>
-      <c r="D20" s="303"/>
-      <c r="E20" s="303"/>
-      <c r="F20" s="303"/>
-      <c r="G20" s="303"/>
+      <c r="B20" s="308"/>
+      <c r="C20" s="308"/>
+      <c r="D20" s="308"/>
+      <c r="E20" s="308"/>
+      <c r="F20" s="308"/>
+      <c r="G20" s="308"/>
       <c r="H20" s="251" t="s">
         <v>755</v>
       </c>
@@ -17465,43 +17621,43 @@
       <c r="X20" s="251"/>
     </row>
     <row r="21" spans="1:24">
-      <c r="A21" s="310" t="s">
+      <c r="A21" s="305" t="s">
         <v>756</v>
       </c>
-      <c r="B21" s="310"/>
-      <c r="C21" s="310"/>
-      <c r="D21" s="310"/>
-      <c r="E21" s="310"/>
-      <c r="F21" s="310"/>
-      <c r="G21" s="310"/>
-      <c r="H21" s="310"/>
-      <c r="I21" s="310"/>
-      <c r="J21" s="310"/>
-      <c r="K21" s="310"/>
-      <c r="L21" s="310"/>
-      <c r="M21" s="310"/>
-      <c r="N21" s="310"/>
-      <c r="O21" s="310"/>
-      <c r="P21" s="310"/>
-      <c r="Q21" s="310"/>
-      <c r="R21" s="310"/>
-      <c r="S21" s="310"/>
-      <c r="T21" s="310"/>
-      <c r="U21" s="310"/>
-      <c r="V21" s="310"/>
-      <c r="W21" s="310"/>
-      <c r="X21" s="310"/>
+      <c r="B21" s="305"/>
+      <c r="C21" s="305"/>
+      <c r="D21" s="305"/>
+      <c r="E21" s="305"/>
+      <c r="F21" s="305"/>
+      <c r="G21" s="305"/>
+      <c r="H21" s="305"/>
+      <c r="I21" s="305"/>
+      <c r="J21" s="305"/>
+      <c r="K21" s="305"/>
+      <c r="L21" s="305"/>
+      <c r="M21" s="305"/>
+      <c r="N21" s="305"/>
+      <c r="O21" s="305"/>
+      <c r="P21" s="305"/>
+      <c r="Q21" s="305"/>
+      <c r="R21" s="305"/>
+      <c r="S21" s="305"/>
+      <c r="T21" s="305"/>
+      <c r="U21" s="305"/>
+      <c r="V21" s="305"/>
+      <c r="W21" s="305"/>
+      <c r="X21" s="305"/>
     </row>
     <row r="22" spans="1:24">
-      <c r="A22" s="304" t="s">
+      <c r="A22" s="309" t="s">
         <v>757</v>
       </c>
-      <c r="B22" s="304"/>
-      <c r="C22" s="304"/>
-      <c r="D22" s="304"/>
-      <c r="E22" s="304"/>
-      <c r="F22" s="304"/>
-      <c r="G22" s="304"/>
+      <c r="B22" s="309"/>
+      <c r="C22" s="309"/>
+      <c r="D22" s="309"/>
+      <c r="E22" s="309"/>
+      <c r="F22" s="309"/>
+      <c r="G22" s="309"/>
       <c r="H22" s="251" t="s">
         <v>758</v>
       </c>
@@ -17523,15 +17679,15 @@
       <c r="X22" s="251"/>
     </row>
     <row r="23" spans="1:24">
-      <c r="A23" s="304" t="s">
+      <c r="A23" s="309" t="s">
         <v>26</v>
       </c>
-      <c r="B23" s="304"/>
-      <c r="C23" s="304"/>
-      <c r="D23" s="304"/>
-      <c r="E23" s="304"/>
-      <c r="F23" s="304"/>
-      <c r="G23" s="304"/>
+      <c r="B23" s="309"/>
+      <c r="C23" s="309"/>
+      <c r="D23" s="309"/>
+      <c r="E23" s="309"/>
+      <c r="F23" s="309"/>
+      <c r="G23" s="309"/>
       <c r="H23" s="251" t="s">
         <v>759</v>
       </c>
@@ -17553,43 +17709,43 @@
       <c r="X23" s="251"/>
     </row>
     <row r="24" spans="1:24">
-      <c r="A24" s="311" t="s">
+      <c r="A24" s="306" t="s">
         <v>760</v>
       </c>
-      <c r="B24" s="311"/>
-      <c r="C24" s="311"/>
-      <c r="D24" s="311"/>
-      <c r="E24" s="311"/>
-      <c r="F24" s="311"/>
-      <c r="G24" s="311"/>
-      <c r="H24" s="311"/>
-      <c r="I24" s="311"/>
-      <c r="J24" s="311"/>
-      <c r="K24" s="311"/>
-      <c r="L24" s="311"/>
-      <c r="M24" s="311"/>
-      <c r="N24" s="311"/>
-      <c r="O24" s="311"/>
-      <c r="P24" s="311"/>
-      <c r="Q24" s="311"/>
-      <c r="R24" s="311"/>
-      <c r="S24" s="311"/>
-      <c r="T24" s="311"/>
-      <c r="U24" s="311"/>
-      <c r="V24" s="311"/>
-      <c r="W24" s="311"/>
-      <c r="X24" s="311"/>
+      <c r="B24" s="306"/>
+      <c r="C24" s="306"/>
+      <c r="D24" s="306"/>
+      <c r="E24" s="306"/>
+      <c r="F24" s="306"/>
+      <c r="G24" s="306"/>
+      <c r="H24" s="306"/>
+      <c r="I24" s="306"/>
+      <c r="J24" s="306"/>
+      <c r="K24" s="306"/>
+      <c r="L24" s="306"/>
+      <c r="M24" s="306"/>
+      <c r="N24" s="306"/>
+      <c r="O24" s="306"/>
+      <c r="P24" s="306"/>
+      <c r="Q24" s="306"/>
+      <c r="R24" s="306"/>
+      <c r="S24" s="306"/>
+      <c r="T24" s="306"/>
+      <c r="U24" s="306"/>
+      <c r="V24" s="306"/>
+      <c r="W24" s="306"/>
+      <c r="X24" s="306"/>
     </row>
     <row r="25" spans="1:24">
-      <c r="A25" s="305" t="s">
+      <c r="A25" s="310" t="s">
         <v>28</v>
       </c>
-      <c r="B25" s="305"/>
-      <c r="C25" s="305"/>
-      <c r="D25" s="305"/>
-      <c r="E25" s="305"/>
-      <c r="F25" s="305"/>
-      <c r="G25" s="305"/>
+      <c r="B25" s="310"/>
+      <c r="C25" s="310"/>
+      <c r="D25" s="310"/>
+      <c r="E25" s="310"/>
+      <c r="F25" s="310"/>
+      <c r="G25" s="310"/>
       <c r="H25" s="251" t="s">
         <v>761</v>
       </c>
@@ -17617,6 +17773,34 @@
     </row>
   </sheetData>
   <mergeCells count="44">
+    <mergeCell ref="A9:G9"/>
+    <mergeCell ref="A10:G10"/>
+    <mergeCell ref="A3:G3"/>
+    <mergeCell ref="A5:G5"/>
+    <mergeCell ref="A6:G6"/>
+    <mergeCell ref="A7:G7"/>
+    <mergeCell ref="A8:G8"/>
+    <mergeCell ref="A20:G20"/>
+    <mergeCell ref="A22:G22"/>
+    <mergeCell ref="A23:G23"/>
+    <mergeCell ref="A25:G25"/>
+    <mergeCell ref="H2:X2"/>
+    <mergeCell ref="H3:X3"/>
+    <mergeCell ref="H6:X6"/>
+    <mergeCell ref="H7:X7"/>
+    <mergeCell ref="H8:X8"/>
+    <mergeCell ref="A11:G11"/>
+    <mergeCell ref="A12:G12"/>
+    <mergeCell ref="A14:G14"/>
+    <mergeCell ref="A15:G15"/>
+    <mergeCell ref="A16:G16"/>
+    <mergeCell ref="A17:G17"/>
+    <mergeCell ref="A2:G2"/>
+    <mergeCell ref="H11:X11"/>
+    <mergeCell ref="H12:X12"/>
+    <mergeCell ref="H14:X14"/>
+    <mergeCell ref="H15:X15"/>
+    <mergeCell ref="A18:G18"/>
     <mergeCell ref="H25:X25"/>
     <mergeCell ref="H5:X5"/>
     <mergeCell ref="A1:X1"/>
@@ -17633,34 +17817,6 @@
     <mergeCell ref="H23:X23"/>
     <mergeCell ref="H9:X9"/>
     <mergeCell ref="H10:X10"/>
-    <mergeCell ref="H11:X11"/>
-    <mergeCell ref="H12:X12"/>
-    <mergeCell ref="H14:X14"/>
-    <mergeCell ref="H15:X15"/>
-    <mergeCell ref="A18:G18"/>
-    <mergeCell ref="A20:G20"/>
-    <mergeCell ref="A22:G22"/>
-    <mergeCell ref="A23:G23"/>
-    <mergeCell ref="A25:G25"/>
-    <mergeCell ref="H2:X2"/>
-    <mergeCell ref="H3:X3"/>
-    <mergeCell ref="H6:X6"/>
-    <mergeCell ref="H7:X7"/>
-    <mergeCell ref="H8:X8"/>
-    <mergeCell ref="A11:G11"/>
-    <mergeCell ref="A12:G12"/>
-    <mergeCell ref="A14:G14"/>
-    <mergeCell ref="A15:G15"/>
-    <mergeCell ref="A16:G16"/>
-    <mergeCell ref="A17:G17"/>
-    <mergeCell ref="A2:G2"/>
-    <mergeCell ref="A9:G9"/>
-    <mergeCell ref="A10:G10"/>
-    <mergeCell ref="A3:G3"/>
-    <mergeCell ref="A5:G5"/>
-    <mergeCell ref="A6:G6"/>
-    <mergeCell ref="A7:G7"/>
-    <mergeCell ref="A8:G8"/>
   </mergeCells>
   <printOptions gridLines="1" gridLinesSet="0"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>